<commit_message>
Python script to find number of cards
</commit_message>
<xml_diff>
--- a/test/Dogs of War.xlsx
+++ b/test/Dogs of War.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="301">
   <si>
     <t>Minions</t>
   </si>
@@ -141,12 +141,6 @@
     <t>Score: make it to the opposite side of the field. Deal damage, if any.</t>
   </si>
   <si>
-    <t>If a card says "regain one health", it means you. Both players start with 20 health.</t>
-  </si>
-  <si>
-    <t>"Forward" is the direction a minion is traveling. "Backwards" is the opposite direction.</t>
-  </si>
-  <si>
     <t>"Adjacent" means either side of the board next to a tower.</t>
   </si>
   <si>
@@ -339,9 +333,6 @@
     <t>Kennel</t>
   </si>
   <si>
-    <t>Reduce the speed of one minion to 0. Any player can pay 4 $ to return its speed to the printed value.</t>
-  </si>
-  <si>
     <t>A Louder Bark</t>
   </si>
   <si>
@@ -384,21 +375,12 @@
     <t>War of the Towers</t>
   </si>
   <si>
-    <t>You and your opponent each pick a tower. Swap the positions of the tower, as well as their control.</t>
-  </si>
-  <si>
     <t>Tower</t>
   </si>
   <si>
     <t>Bone Pile</t>
   </si>
   <si>
-    <t>If there is only one minion adjacent to this tower, decrease the speed of that minion by 1.</t>
-  </si>
-  <si>
-    <t>Place an eye token on any empty square on your side of the board. This tower is considered to be adjacent to the token. Remove the token when this tower is destroyed.</t>
-  </si>
-  <si>
     <t>Howl</t>
   </si>
   <si>
@@ -711,9 +693,6 @@
     <t>Thorn</t>
   </si>
   <si>
-    <t>If this card has a valid enemy target and does not attack, gain 2 $</t>
-  </si>
-  <si>
     <t>Worse than the Bark</t>
   </si>
   <si>
@@ -738,9 +717,6 @@
     <t>Greyfriars Bobby</t>
   </si>
   <si>
-    <t>Regain 1 health each turn.</t>
-  </si>
-  <si>
     <t>Loyalty Pup</t>
   </si>
   <si>
@@ -916,6 +892,45 @@
   </si>
   <si>
     <t>Maybe each player places 4 tiles</t>
+  </si>
+  <si>
+    <t>Reduce the speed of one minion to 0. Any player can pay 2 $ to return its speed to the printed value.</t>
+  </si>
+  <si>
+    <t>make tiles double width</t>
+  </si>
+  <si>
+    <t>If a card says "regain one health", it means you. Both players start with 10 health.</t>
+  </si>
+  <si>
+    <t>When you start your turn with Greyfriar's Bobby in play, regain one health.</t>
+  </si>
+  <si>
+    <t>Blue dogs that affect others--if end on same space, heal/damage depending on alignment?</t>
+  </si>
+  <si>
+    <t>You can choose the order that minions move on your turn</t>
+  </si>
+  <si>
+    <t>Whenever a minion ends its movement adjacent to this tower, if it is the only minion adjacent to this tower, decrease the speed of that minion by 1.</t>
+  </si>
+  <si>
+    <t>If this card has a valid enemy target and does not attack, gain 4 $</t>
+  </si>
+  <si>
+    <t>Choose one of your opponent's towers. Your opponent chooses one of your towers. Swap the positions of the towers, as well as their control.</t>
+  </si>
+  <si>
+    <t>Place an eye token in any empty space on your side of the board. Squares adjacent to the token are also adjacent to the tower. Remove the token when this tower is destroyed.</t>
+  </si>
+  <si>
+    <t>Every Dog, Every Day</t>
+  </si>
+  <si>
+    <t>Gain 2 $</t>
+  </si>
+  <si>
+    <t>Upgrade</t>
   </si>
 </sst>
 </file>
@@ -972,7 +987,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -980,6 +995,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1296,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="77" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1462,7 +1478,7 @@
         <v>17</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
@@ -1472,7 +1488,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="K8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
@@ -1492,33 +1508,36 @@
         <v>10</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="G12" s="2" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="J13" s="2" t="s">
-        <v>37</v>
+      <c r="A13" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="E14" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>38</v>
+        <v>164</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="E15" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>36</v>
@@ -1531,7 +1550,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J17" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.45">
@@ -1539,7 +1558,7 @@
         <v>24</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.45">
@@ -1582,25 +1601,31 @@
         <v>33</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="G24" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>292</v>
       </c>
       <c r="Q24" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="D25" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q25" s="2" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="Q25" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="Q26" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.45">
@@ -1608,7 +1633,7 @@
         <v>13</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.45">
@@ -1616,23 +1641,23 @@
         <v>14</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>16</v>
@@ -1640,7 +1665,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>22</v>
@@ -1648,21 +1673,21 @@
     </row>
     <row r="32" spans="1:17" ht="111" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="Q33" s="2" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.45">
@@ -1670,7 +1695,7 @@
         <v>29</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.45">
@@ -1680,47 +1705,47 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.45">
       <c r="G36" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.45">
       <c r="M37" s="2" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.45">
       <c r="G39" s="2" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.45">
       <c r="G40" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B45" s="2">
         <v>10</v>
@@ -1729,12 +1754,12 @@
         <v>5</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B46" s="2">
         <v>6</v>
@@ -1743,12 +1768,12 @@
         <v>5</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B47" s="2">
         <v>4</v>
@@ -1757,7 +1782,7 @@
         <v>5</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1767,11 +1792,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1782,147 +1807,141 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>159</v>
       </c>
       <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>271</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" t="s">
+        <v>271</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>272</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>241</v>
       </c>
       <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>271</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>242</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>224</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -1930,1840 +1949,1981 @@
         <v>85</v>
       </c>
       <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" t="s">
+        <v>271</v>
       </c>
       <c r="F6" t="s">
         <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>173</v>
       </c>
       <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>279</v>
-      </c>
-      <c r="F7" t="s">
-        <v>88</v>
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>174</v>
       </c>
       <c r="H7" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>149</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
+      <c r="C8" t="s">
+        <v>271</v>
+      </c>
       <c r="D8" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="H8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>170</v>
       </c>
       <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>279</v>
-      </c>
-      <c r="F9" t="s">
-        <v>93</v>
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>169</v>
       </c>
       <c r="H9" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>207</v>
       </c>
       <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>279</v>
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>276</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>174</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="I10" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
         <v>6</v>
       </c>
-      <c r="D11" t="s">
-        <v>279</v>
+      <c r="E11">
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="H11" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
         <v>5</v>
       </c>
-      <c r="D12" t="s">
-        <v>279</v>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>273</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="H12" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I12" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>226</v>
       </c>
       <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>279</v>
-      </c>
-      <c r="F13" t="s">
-        <v>101</v>
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>224</v>
       </c>
       <c r="H13" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I13" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>188</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>271</v>
       </c>
       <c r="D14" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>174</v>
       </c>
       <c r="H14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I14" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>279</v>
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H15" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="I15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="D16" t="s">
-        <v>279</v>
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="H16" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I16" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>233</v>
       </c>
       <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>279</v>
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>271</v>
       </c>
       <c r="F17" t="s">
-        <v>107</v>
+        <v>234</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>224</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I17" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="B18">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>279</v>
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
+        <v>174</v>
       </c>
       <c r="H18" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I18" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
+      <c r="C19" t="s">
+        <v>271</v>
+      </c>
       <c r="D19" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F19" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="G19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B20">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>279</v>
-      </c>
-      <c r="F20" t="s">
-        <v>114</v>
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="H20" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I20" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>271</v>
       </c>
       <c r="D21" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F21" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>190</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>271</v>
       </c>
       <c r="D22" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>191</v>
       </c>
       <c r="G22" t="s">
-        <v>69</v>
+        <v>174</v>
       </c>
       <c r="H22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I22" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>271</v>
+      </c>
+      <c r="D23" t="s">
+        <v>271</v>
       </c>
       <c r="F23" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="G23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H23" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="I23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>243</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>271</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>122</v>
+        <v>244</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>224</v>
       </c>
       <c r="H24" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I24" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>280</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>271</v>
+      </c>
+      <c r="D25" t="s">
+        <v>271</v>
+      </c>
+      <c r="F25" t="s">
+        <v>154</v>
+      </c>
+      <c r="G25" t="s">
         <v>123</v>
       </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="H25" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" t="s">
         <v>124</v>
-      </c>
-      <c r="G25" t="s">
-        <v>69</v>
-      </c>
-      <c r="H25" t="s">
-        <v>119</v>
-      </c>
-      <c r="I25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="B26">
         <v>4</v>
       </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
       <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
         <v>0</v>
       </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
       <c r="F26" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H26" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="I26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>271</v>
+      </c>
+      <c r="D27" t="s">
+        <v>271</v>
       </c>
       <c r="F27" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="G27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H27" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="I27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="B28">
         <v>5</v>
       </c>
-      <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28">
-        <v>6</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
+      <c r="C28" t="s">
+        <v>271</v>
+      </c>
+      <c r="D28" t="s">
+        <v>271</v>
+      </c>
+      <c r="F28" t="s">
+        <v>97</v>
       </c>
       <c r="G28" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="H28" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I28" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>271</v>
+      </c>
+      <c r="D29" t="s">
+        <v>271</v>
       </c>
       <c r="F29" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="G29" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H29" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I29" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-      <c r="D30">
-        <v>5</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>271</v>
+      </c>
+      <c r="D30" t="s">
+        <v>271</v>
       </c>
       <c r="F30" t="s">
-        <v>281</v>
+        <v>171</v>
       </c>
       <c r="G30" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
       <c r="H30" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I30" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>245</v>
       </c>
       <c r="B31">
-        <v>7</v>
-      </c>
-      <c r="C31">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>271</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>136</v>
+        <v>246</v>
       </c>
       <c r="G31" t="s">
-        <v>129</v>
+        <v>224</v>
       </c>
       <c r="H31" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I31" t="s">
-        <v>130</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>247</v>
       </c>
       <c r="B32">
         <v>5</v>
       </c>
-      <c r="C32">
-        <v>3</v>
+      <c r="C32" t="s">
+        <v>271</v>
       </c>
       <c r="D32">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>248</v>
       </c>
       <c r="G32" t="s">
-        <v>129</v>
+        <v>224</v>
       </c>
       <c r="H32" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I32" t="s">
-        <v>130</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="B33">
-        <v>6</v>
-      </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-      <c r="D33">
-        <v>4</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>271</v>
+      </c>
+      <c r="D33" t="s">
+        <v>271</v>
       </c>
       <c r="F33" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="G33" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H33" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I33" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>140</v>
+        <v>193</v>
       </c>
       <c r="B34">
-        <v>7</v>
-      </c>
-      <c r="C34">
-        <v>4</v>
-      </c>
-      <c r="D34">
-        <v>11</v>
-      </c>
-      <c r="E34">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>271</v>
+      </c>
+      <c r="D34" t="s">
+        <v>271</v>
       </c>
       <c r="F34" t="s">
-        <v>286</v>
+        <v>194</v>
       </c>
       <c r="G34" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="H34" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I34" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="B35">
-        <v>5</v>
-      </c>
-      <c r="C35">
-        <v>4</v>
-      </c>
-      <c r="D35">
-        <v>6</v>
-      </c>
-      <c r="E35">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" t="s">
+        <v>271</v>
       </c>
       <c r="F35" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="G35" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="H35" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I35" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>18</v>
       </c>
       <c r="B36">
-        <v>4</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>271</v>
       </c>
       <c r="D36">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
+      <c r="F36" t="s">
+        <v>297</v>
+      </c>
       <c r="G36" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="H36" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I36" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>271</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
       <c r="H37" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I37" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>145</v>
+        <v>178</v>
       </c>
       <c r="B38">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>147</v>
+        <v>179</v>
       </c>
       <c r="G38" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="H38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I38" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>208</v>
       </c>
       <c r="B39">
-        <v>8</v>
-      </c>
-      <c r="C39">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>271</v>
       </c>
       <c r="D39">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>149</v>
+        <v>209</v>
       </c>
       <c r="G39" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="H39" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I39" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>150</v>
+        <v>227</v>
       </c>
       <c r="B40">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C40">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
       <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40" t="s">
-        <v>282</v>
+        <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>129</v>
+        <v>224</v>
       </c>
       <c r="H40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I40" t="s">
-        <v>130</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>228</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>3</v>
       </c>
       <c r="D41">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>152</v>
+        <v>291</v>
       </c>
       <c r="G41" t="s">
-        <v>129</v>
+        <v>224</v>
       </c>
       <c r="H41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I41" t="s">
-        <v>130</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>153</v>
+        <v>210</v>
       </c>
       <c r="B42">
-        <v>3</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>271</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="G42" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="H42" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I42" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43">
         <v>4</v>
       </c>
-      <c r="D43" t="s">
-        <v>279</v>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="G43" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H43" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I43" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>157</v>
+        <v>235</v>
       </c>
       <c r="B44">
-        <v>3</v>
-      </c>
-      <c r="D44" t="s">
-        <v>279</v>
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>271</v>
       </c>
       <c r="F44" t="s">
-        <v>158</v>
+        <v>236</v>
       </c>
       <c r="G44" t="s">
-        <v>129</v>
+        <v>224</v>
       </c>
       <c r="H44" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I44" t="s">
-        <v>130</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>288</v>
+        <v>79</v>
       </c>
       <c r="B45">
         <v>5</v>
       </c>
-      <c r="D45" t="s">
-        <v>279</v>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>160</v>
+        <v>77</v>
       </c>
       <c r="G45" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="H45" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I45" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>161</v>
+        <v>78</v>
       </c>
       <c r="B46">
         <v>3</v>
       </c>
-      <c r="D46" t="s">
-        <v>279</v>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>162</v>
+        <v>80</v>
       </c>
       <c r="G46" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="H46" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I46" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47">
         <v>6</v>
       </c>
-      <c r="D47" t="s">
-        <v>279</v>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="G47" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="H47" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I47" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="B48">
-        <v>5</v>
-      </c>
-      <c r="D48">
-        <v>3</v>
-      </c>
-      <c r="E48">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>271</v>
+      </c>
+      <c r="D48" t="s">
+        <v>271</v>
       </c>
       <c r="F48" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
       <c r="G48" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="H48" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="I48" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>271</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F49" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="G49" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="H49" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I49" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>169</v>
+        <v>212</v>
       </c>
       <c r="B50">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>271</v>
       </c>
       <c r="D50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F50" t="s">
+        <v>213</v>
       </c>
       <c r="G50" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="H50" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I50" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>171</v>
+        <v>100</v>
       </c>
       <c r="B51">
         <v>8</v>
       </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51">
-        <v>3</v>
+      <c r="C51" t="s">
+        <v>271</v>
+      </c>
+      <c r="D51" t="s">
+        <v>271</v>
       </c>
       <c r="F51" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="G51" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="H51" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="I51" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="B52">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E52">
         <v>2</v>
       </c>
       <c r="F52" t="s">
-        <v>173</v>
+        <v>278</v>
       </c>
       <c r="G52" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H52" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="I52" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>237</v>
       </c>
       <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>3</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>271</v>
+      </c>
+      <c r="F53" t="s">
+        <v>238</v>
       </c>
       <c r="G53" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="H53" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I53" t="s">
-        <v>174</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="D54" t="s">
-        <v>279</v>
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>271</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="G54" t="s">
-        <v>175</v>
+        <v>123</v>
       </c>
       <c r="H54" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="I54" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>178</v>
+        <v>249</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>271</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>250</v>
       </c>
       <c r="G55" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="H55" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I55" t="s">
-        <v>174</v>
+        <v>225</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>179</v>
+        <v>251</v>
       </c>
       <c r="B56">
-        <v>5</v>
-      </c>
-      <c r="C56">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>271</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E56">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>252</v>
       </c>
       <c r="G56" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="H56" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I56" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="B57">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D57">
         <v>3</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c r="G57" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="H57" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I57" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>184</v>
+        <v>102</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>3</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
+      <c r="C58" t="s">
+        <v>271</v>
+      </c>
+      <c r="D58" t="s">
+        <v>271</v>
       </c>
       <c r="F58" t="s">
-        <v>185</v>
+        <v>103</v>
       </c>
       <c r="G58" t="s">
-        <v>180</v>
+        <v>67</v>
       </c>
       <c r="H58" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I58" t="s">
-        <v>181</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
       <c r="B59">
-        <v>5</v>
-      </c>
-      <c r="C59">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>271</v>
       </c>
       <c r="D59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>187</v>
+        <v>217</v>
       </c>
       <c r="G59" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H59" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I59" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>188</v>
+        <v>135</v>
       </c>
       <c r="B60">
         <v>5</v>
       </c>
       <c r="C60">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D60">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E60">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F60" t="s">
+        <v>136</v>
       </c>
       <c r="G60" t="s">
-        <v>180</v>
+        <v>123</v>
       </c>
       <c r="H60" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I60" t="s">
-        <v>181</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="B61">
-        <v>3</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>271</v>
       </c>
       <c r="D61">
         <v>3</v>
       </c>
       <c r="E61">
-        <v>2</v>
-      </c>
-      <c r="F61" t="s">
-        <v>201</v>
+        <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>180</v>
+        <v>123</v>
       </c>
       <c r="H61" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I61" t="s">
-        <v>181</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D62">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E62">
         <v>1</v>
       </c>
-      <c r="F62" t="s">
-        <v>191</v>
-      </c>
       <c r="G62" t="s">
-        <v>180</v>
+        <v>123</v>
       </c>
       <c r="H62" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I62" t="s">
-        <v>181</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>192</v>
+        <v>253</v>
       </c>
       <c r="B63">
-        <v>6</v>
-      </c>
-      <c r="C63">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C63" t="s">
+        <v>271</v>
       </c>
       <c r="D63">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E63">
         <v>2</v>
       </c>
       <c r="F63" t="s">
-        <v>193</v>
+        <v>254</v>
       </c>
       <c r="G63" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="H63" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I63" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>194</v>
+        <v>105</v>
       </c>
       <c r="B64">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>271</v>
       </c>
       <c r="D64" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F64" t="s">
-        <v>195</v>
+        <v>104</v>
       </c>
       <c r="G64" t="s">
-        <v>180</v>
+        <v>67</v>
       </c>
       <c r="H64" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I64" t="s">
-        <v>181</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>196</v>
+        <v>255</v>
       </c>
       <c r="B65">
-        <v>3</v>
-      </c>
-      <c r="D65" t="s">
-        <v>279</v>
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>271</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
       </c>
       <c r="F65" t="s">
-        <v>197</v>
+        <v>256</v>
       </c>
       <c r="G65" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="H65" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="I65" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>199</v>
+        <v>257</v>
       </c>
       <c r="B66">
-        <v>6</v>
-      </c>
-      <c r="D66" t="s">
-        <v>279</v>
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>271</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>200</v>
+        <v>258</v>
       </c>
       <c r="G66" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="H66" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="I66" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>202</v>
+        <v>81</v>
       </c>
       <c r="B67">
-        <v>3</v>
-      </c>
-      <c r="D67" t="s">
-        <v>279</v>
+        <v>2</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>203</v>
+        <v>82</v>
       </c>
       <c r="G67" t="s">
-        <v>180</v>
+        <v>67</v>
       </c>
       <c r="H67" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I67" t="s">
-        <v>181</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>204</v>
+        <v>106</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C68" t="s">
+        <v>271</v>
       </c>
       <c r="D68" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F68" t="s">
-        <v>205</v>
+        <v>107</v>
       </c>
       <c r="G68" t="s">
-        <v>180</v>
+        <v>67</v>
       </c>
       <c r="H68" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I68" t="s">
-        <v>181</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="B69">
+        <v>5</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
         <v>6</v>
       </c>
-      <c r="D69" t="s">
-        <v>279</v>
+      <c r="E69">
+        <v>2</v>
       </c>
       <c r="F69" t="s">
-        <v>208</v>
+        <v>140</v>
       </c>
       <c r="G69" t="s">
-        <v>180</v>
+        <v>123</v>
       </c>
       <c r="H69" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I69" t="s">
-        <v>181</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>209</v>
+        <v>139</v>
       </c>
       <c r="B70">
+        <v>5</v>
+      </c>
+      <c r="C70">
         <v>4</v>
       </c>
-      <c r="D70" t="s">
-        <v>279</v>
+      <c r="D70">
+        <v>7</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>210</v>
+        <v>141</v>
       </c>
       <c r="G70" t="s">
-        <v>180</v>
+        <v>123</v>
       </c>
       <c r="H70" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I70" t="s">
-        <v>181</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="B71">
-        <v>2</v>
-      </c>
-      <c r="D71" t="s">
-        <v>279</v>
-      </c>
-      <c r="F71" t="s">
-        <v>212</v>
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+      <c r="D71">
+        <v>4</v>
+      </c>
+      <c r="E71">
+        <v>3</v>
       </c>
       <c r="G71" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H71" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I71" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="B72">
         <v>3</v>
       </c>
-      <c r="D72">
-        <v>1</v>
-      </c>
-      <c r="E72">
-        <v>0</v>
+      <c r="C72" t="s">
+        <v>271</v>
+      </c>
+      <c r="D72" t="s">
+        <v>271</v>
       </c>
       <c r="F72" t="s">
-        <v>284</v>
+        <v>199</v>
       </c>
       <c r="G72" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H72" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="I72" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>214</v>
+        <v>157</v>
       </c>
       <c r="B73">
         <v>6</v>
       </c>
-      <c r="D73">
-        <v>1</v>
-      </c>
-      <c r="E73">
-        <v>1</v>
+      <c r="C73" t="s">
+        <v>271</v>
+      </c>
+      <c r="D73" t="s">
+        <v>271</v>
       </c>
       <c r="F73" t="s">
-        <v>215</v>
+        <v>158</v>
       </c>
       <c r="G73" t="s">
-        <v>180</v>
+        <v>123</v>
       </c>
       <c r="H73" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="I73" t="s">
-        <v>181</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="B74">
-        <v>6</v>
-      </c>
-      <c r="D74">
-        <v>2</v>
-      </c>
-      <c r="E74">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C74" t="s">
+        <v>271</v>
       </c>
       <c r="F74" t="s">
-        <v>217</v>
+        <v>279</v>
       </c>
       <c r="G74" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="H74" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="I74" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="B75">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C75">
+        <v>6</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E75">
         <v>1</v>
       </c>
       <c r="F75" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="G75" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="H75" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="I75" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B76">
         <v>3</v>
       </c>
+      <c r="C76" t="s">
+        <v>271</v>
+      </c>
       <c r="D76">
         <v>1</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F76" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G76" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H76" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I76" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>221</v>
+        <v>183</v>
       </c>
       <c r="B77">
         <v>3</v>
       </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
       <c r="D77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E77">
         <v>2</v>
       </c>
       <c r="F77" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="G77" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H77" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="I77" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C78" t="s">
+        <v>271</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -3772,697 +3932,795 @@
         <v>0</v>
       </c>
       <c r="F78" t="s">
+        <v>260</v>
+      </c>
+      <c r="G78" t="s">
+        <v>224</v>
+      </c>
+      <c r="H78" t="s">
+        <v>115</v>
+      </c>
+      <c r="I78" t="s">
         <v>225</v>
-      </c>
-      <c r="G78" t="s">
-        <v>180</v>
-      </c>
-      <c r="H78" t="s">
-        <v>119</v>
-      </c>
-      <c r="I78" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>226</v>
+        <v>184</v>
       </c>
       <c r="B79">
         <v>2</v>
       </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
       <c r="D79">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E79">
         <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>227</v>
+        <v>185</v>
       </c>
       <c r="G79" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H79" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="I79" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>228</v>
+        <v>201</v>
       </c>
       <c r="B80">
         <v>6</v>
       </c>
-      <c r="D80">
-        <v>2</v>
-      </c>
-      <c r="E80">
-        <v>2</v>
+      <c r="C80" t="s">
+        <v>271</v>
+      </c>
+      <c r="D80" t="s">
+        <v>271</v>
+      </c>
+      <c r="F80" t="s">
+        <v>202</v>
       </c>
       <c r="G80" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H80" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="I80" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>233</v>
+        <v>261</v>
       </c>
       <c r="B81">
-        <v>3</v>
-      </c>
-      <c r="C81">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C81" t="s">
+        <v>271</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F81" t="s">
+        <v>262</v>
       </c>
       <c r="G81" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="H81" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I81" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>234</v>
+        <v>263</v>
       </c>
       <c r="B82">
-        <v>8</v>
-      </c>
-      <c r="C82">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C82" t="s">
+        <v>271</v>
       </c>
       <c r="D82">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E82">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F82" t="s">
+        <v>264</v>
       </c>
       <c r="G82" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="H82" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I82" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>235</v>
+        <v>265</v>
       </c>
       <c r="B83">
         <v>4</v>
       </c>
-      <c r="C83">
-        <v>3</v>
+      <c r="C83" t="s">
+        <v>271</v>
       </c>
       <c r="D83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F83" t="s">
-        <v>236</v>
+        <v>266</v>
       </c>
       <c r="G83" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="H83" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I83" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>237</v>
+        <v>108</v>
       </c>
       <c r="B84">
-        <v>5</v>
-      </c>
-      <c r="C84">
-        <v>6</v>
-      </c>
-      <c r="D84">
-        <v>3</v>
-      </c>
-      <c r="E84">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="C84" t="s">
+        <v>271</v>
+      </c>
+      <c r="D84" t="s">
+        <v>271</v>
       </c>
       <c r="F84" t="s">
-        <v>238</v>
+        <v>109</v>
       </c>
       <c r="G84" t="s">
-        <v>231</v>
+        <v>67</v>
       </c>
       <c r="H84" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I84" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>239</v>
+        <v>267</v>
       </c>
       <c r="B85">
         <v>5</v>
       </c>
-      <c r="C85">
-        <v>4</v>
+      <c r="C85" t="s">
+        <v>271</v>
       </c>
       <c r="D85">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E85">
         <v>1</v>
       </c>
       <c r="F85" t="s">
-        <v>240</v>
+        <v>268</v>
       </c>
       <c r="G85" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="H85" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="I85" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>241</v>
+        <v>142</v>
       </c>
       <c r="B86">
+        <v>8</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86">
+        <v>8</v>
+      </c>
+      <c r="E86">
         <v>3</v>
       </c>
       <c r="F86" t="s">
-        <v>242</v>
+        <v>143</v>
       </c>
       <c r="G86" t="s">
-        <v>231</v>
+        <v>123</v>
       </c>
       <c r="H86" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I86" t="s">
-        <v>232</v>
+        <v>124</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>243</v>
+        <v>203</v>
       </c>
       <c r="B87">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C87" t="s">
+        <v>271</v>
+      </c>
+      <c r="D87" t="s">
+        <v>271</v>
       </c>
       <c r="F87" t="s">
-        <v>244</v>
+        <v>204</v>
       </c>
       <c r="G87" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="H87" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I87" t="s">
-        <v>232</v>
+        <v>175</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B88">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C88" t="s">
+        <v>271</v>
       </c>
       <c r="F88" t="s">
-        <v>246</v>
+        <v>277</v>
       </c>
       <c r="G88" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="H88" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I88" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>247</v>
+        <v>83</v>
       </c>
       <c r="B89">
         <v>5</v>
       </c>
+      <c r="C89">
+        <v>5</v>
+      </c>
+      <c r="D89">
+        <v>3</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
       <c r="F89" t="s">
-        <v>287</v>
+        <v>84</v>
       </c>
       <c r="G89" t="s">
-        <v>231</v>
+        <v>67</v>
       </c>
       <c r="H89" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="I89" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>248</v>
+        <v>205</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C90" t="s">
+        <v>271</v>
+      </c>
+      <c r="D90" t="s">
+        <v>271</v>
       </c>
       <c r="F90" t="s">
-        <v>285</v>
+        <v>206</v>
       </c>
       <c r="G90" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="H90" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I90" t="s">
-        <v>232</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>249</v>
+        <v>110</v>
       </c>
       <c r="B91">
-        <v>2</v>
-      </c>
-      <c r="D91">
-        <v>2</v>
-      </c>
-      <c r="E91">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="C91" t="s">
+        <v>271</v>
+      </c>
+      <c r="D91" t="s">
+        <v>271</v>
       </c>
       <c r="F91" t="s">
-        <v>250</v>
+        <v>111</v>
       </c>
       <c r="G91" t="s">
-        <v>231</v>
+        <v>67</v>
       </c>
       <c r="H91" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="I91" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>251</v>
+        <v>119</v>
       </c>
       <c r="B92">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C92" t="s">
+        <v>271</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92">
         <v>2</v>
       </c>
       <c r="F92" t="s">
-        <v>252</v>
+        <v>120</v>
       </c>
       <c r="G92" t="s">
-        <v>231</v>
+        <v>67</v>
       </c>
       <c r="H92" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I92" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>253</v>
+        <v>165</v>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C93" t="s">
+        <v>271</v>
       </c>
       <c r="D93">
         <v>1</v>
       </c>
       <c r="E93">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F93" t="s">
-        <v>254</v>
+        <v>275</v>
       </c>
       <c r="G93" t="s">
-        <v>231</v>
+        <v>123</v>
       </c>
       <c r="H93" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I93" t="s">
-        <v>232</v>
+        <v>124</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>255</v>
+        <v>121</v>
       </c>
       <c r="B94">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C94" t="s">
+        <v>271</v>
       </c>
       <c r="D94">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E94">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F94" t="s">
-        <v>256</v>
+        <v>122</v>
       </c>
       <c r="G94" t="s">
-        <v>231</v>
+        <v>67</v>
       </c>
       <c r="H94" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I94" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>257</v>
+        <v>144</v>
       </c>
       <c r="B95">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="C95">
+        <v>6</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="G95" t="s">
-        <v>231</v>
+        <v>123</v>
       </c>
       <c r="H95" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="I95" t="s">
-        <v>232</v>
+        <v>124</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>259</v>
+        <v>166</v>
       </c>
       <c r="B96">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C96" t="s">
+        <v>271</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F96" t="s">
-        <v>260</v>
+        <v>167</v>
       </c>
       <c r="G96" t="s">
-        <v>231</v>
+        <v>123</v>
       </c>
       <c r="H96" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I96" t="s">
-        <v>232</v>
+        <v>124</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>261</v>
+        <v>218</v>
       </c>
       <c r="B97">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>271</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F97" t="s">
-        <v>262</v>
+        <v>219</v>
       </c>
       <c r="G97" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="H97" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I97" t="s">
-        <v>232</v>
+        <v>175</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>263</v>
+        <v>145</v>
       </c>
       <c r="B98">
+        <v>6</v>
+      </c>
+      <c r="C98">
         <v>2</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E98">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>264</v>
+        <v>146</v>
       </c>
       <c r="G98" t="s">
-        <v>231</v>
+        <v>123</v>
       </c>
       <c r="H98" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="I98" t="s">
-        <v>232</v>
+        <v>124</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="B99">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>271</v>
       </c>
       <c r="D99">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F99" t="s">
-        <v>266</v>
+        <v>295</v>
       </c>
       <c r="G99" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="H99" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I99" t="s">
-        <v>232</v>
+        <v>175</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>267</v>
+        <v>113</v>
       </c>
       <c r="B100">
         <v>3</v>
       </c>
-      <c r="D100">
-        <v>0</v>
-      </c>
-      <c r="E100">
-        <v>0</v>
+      <c r="C100" t="s">
+        <v>271</v>
+      </c>
+      <c r="D100" t="s">
+        <v>271</v>
       </c>
       <c r="F100" t="s">
-        <v>268</v>
+        <v>112</v>
       </c>
       <c r="G100" t="s">
-        <v>231</v>
+        <v>67</v>
       </c>
       <c r="H100" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="I100" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>269</v>
+        <v>186</v>
       </c>
       <c r="B101">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E101">
         <v>2</v>
       </c>
       <c r="F101" t="s">
-        <v>270</v>
+        <v>187</v>
       </c>
       <c r="G101" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="H101" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="I101" t="s">
-        <v>232</v>
+        <v>175</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>271</v>
+        <v>147</v>
       </c>
       <c r="B102">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C102">
+        <v>3</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E102">
         <v>2</v>
       </c>
       <c r="F102" t="s">
-        <v>272</v>
+        <v>148</v>
       </c>
       <c r="G102" t="s">
-        <v>231</v>
+        <v>123</v>
       </c>
       <c r="H102" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="I102" t="s">
-        <v>232</v>
+        <v>124</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>273</v>
+        <v>114</v>
       </c>
       <c r="B103">
-        <v>4</v>
-      </c>
-      <c r="D103">
-        <v>1</v>
-      </c>
-      <c r="E103">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="C103" t="s">
+        <v>271</v>
+      </c>
+      <c r="D103" t="s">
+        <v>271</v>
       </c>
       <c r="F103" t="s">
-        <v>274</v>
+        <v>296</v>
       </c>
       <c r="G103" t="s">
-        <v>231</v>
+        <v>67</v>
       </c>
       <c r="H103" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="I103" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B104">
         <v>5</v>
       </c>
+      <c r="C104" t="s">
+        <v>271</v>
+      </c>
       <c r="D104">
         <v>1</v>
       </c>
       <c r="E104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G104" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="H104" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I104" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>277</v>
+        <v>221</v>
       </c>
       <c r="B105">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C105" t="s">
+        <v>271</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E105">
-        <v>0</v>
-      </c>
-      <c r="F105" t="s">
-        <v>278</v>
+        <v>2</v>
       </c>
       <c r="G105" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="H105" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I105" t="s">
-        <v>232</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>298</v>
+      </c>
+      <c r="B106">
+        <v>3</v>
+      </c>
+      <c r="F106" t="s">
+        <v>299</v>
+      </c>
+      <c r="G106" t="s">
+        <v>169</v>
+      </c>
+      <c r="H106" t="s">
+        <v>87</v>
+      </c>
+      <c r="I106" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I105">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>